<commit_message>
[ADD] new addons, update 21.12
</commit_message>
<xml_diff>
--- a/import_template_product/tests/sample_selection_type_error.xlsx
+++ b/import_template_product/tests/sample_selection_type_error.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t xml:space="preserve">default_code</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">Product 6 test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROD7TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 7 test</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,12 +167,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,16 +211,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,28 +230,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:I1"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
@@ -265,8 +261,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,16 +297,16 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -323,7 +318,7 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -331,16 +326,16 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -352,7 +347,7 @@
       <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -360,16 +355,16 @@
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -381,7 +376,7 @@
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -389,16 +384,16 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -410,7 +405,7 @@
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -418,16 +413,16 @@
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -439,7 +434,7 @@
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -447,16 +442,16 @@
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -465,14 +460,40 @@
       <c r="H7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>